<commit_message>
Alert msg validation added and unwanted code removed
</commit_message>
<xml_diff>
--- a/Data/Result/ResAPPaytoInsr.xlsx
+++ b/Data/Result/ResAPPaytoInsr.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
   <si>
     <t>TestId</t>
   </si>
@@ -50,6 +50,12 @@
   </si>
   <si>
     <t>EAPV21-0167</t>
+  </si>
+  <si>
+    <t>EAPV21-0168</t>
+  </si>
+  <si>
+    <t>EAPV21-0169</t>
   </si>
 </sst>
 </file>
@@ -414,7 +420,7 @@
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>